<commit_message>
docs: add rule for control device with neuron
</commit_message>
<xml_diff>
--- a/developer-scripts/neuron_batch_modbus_5.xlsx
+++ b/developer-scripts/neuron_batch_modbus_5.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rockyjin/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rockyjin/Downloads/workspace/edge/src/edge-stack/developer-scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
   <si>
     <t>objn</t>
   </si>
@@ -116,6 +116,10 @@
   </si>
   <si>
     <t>1!400005</t>
+  </si>
+  <si>
+    <t>RW</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1361,7 +1365,7 @@
   <dimension ref="A1:O1001"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1635,7 +1639,7 @@
         <v>1</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="N6" s="4">
         <v>0</v>

</xml_diff>